<commit_message>
update sanpham thêm lọc theo nhà sx và thay đổi 1 số cấu trúc gui/F_SanPham.form thêm ISanPhamService dổi tên ISanPhamService.java > ISanPhamChiTietService.java
</commit_message>
<xml_diff>
--- a/Dien_May_Do/src/com/dienmaydo/excel/SPCT.xlsx
+++ b/Dien_May_Do/src/com/dienmaydo/excel/SPCT.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
   <si>
     <t/>
   </si>
@@ -59,6 +59,9 @@
     <t>Mô Tả</t>
   </si>
   <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
     <t>SPCT01</t>
   </si>
   <si>
@@ -83,6 +86,30 @@
     <t>No Mô Tả</t>
   </si>
   <si>
+    <t>Ngừng kinh doanh</t>
+  </si>
+  <si>
+    <t>SPCT011</t>
+  </si>
+  <si>
+    <t>AH-X9XEW1</t>
+  </si>
+  <si>
+    <t>Phổ biến</t>
+  </si>
+  <si>
+    <t>Nâu</t>
+  </si>
+  <si>
+    <t>82.0 - 20.5 - 48.2</t>
+  </si>
+  <si>
+    <t>Sắt không gỉ</t>
+  </si>
+  <si>
+    <t>Đang kinh doanh</t>
+  </si>
+  <si>
     <t>SPCT02</t>
   </si>
   <si>
@@ -107,9 +134,6 @@
     <t>KG50F62</t>
   </si>
   <si>
-    <t>Phổ biến</t>
-  </si>
-  <si>
     <t>70.0 - 30.0 - 25.5</t>
   </si>
   <si>
@@ -176,9 +200,6 @@
     <t>40.0 - 20.0 - 70.0</t>
   </si>
   <si>
-    <t>Sắt không gỉ</t>
-  </si>
-  <si>
     <t>mayhutbui.png</t>
   </si>
   <si>
@@ -198,9 +219,6 @@
   </si>
   <si>
     <t>EWE451LB-DPX2</t>
-  </si>
-  <si>
-    <t>82.0 - 20.5 - 48.2</t>
   </si>
   <si>
     <t>binhnonglanh.png</t>
@@ -211,13 +229,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -248,7 +271,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A3:M13"/>
+  <dimension ref="A3:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -299,16 +322,19 @@
       <c r="M4" t="s">
         <v>14</v>
       </c>
+      <c r="N4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" ht="20.0" customHeight="true">
       <c r="A5" t="n">
         <v>1.0</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" t="n">
         <v>100.0</v>
@@ -320,25 +346,28 @@
         <v>3000.0</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" t="n">
         <v>20.0</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M5" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" ht="20.0" customHeight="true">
@@ -346,40 +375,43 @@
         <v>2.0</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6" t="n">
-        <v>1000.0</v>
+        <v>32.0</v>
       </c>
       <c r="E6" t="n">
-        <v>2500.0</v>
+        <v>141200.0</v>
       </c>
       <c r="F6" t="n">
-        <v>4000.0</v>
+        <v>54300.0</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I6" t="n">
-        <v>2.0</v>
+        <v>20.0</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="M6" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="N6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="20.0" customHeight="true">
@@ -387,40 +419,43 @@
         <v>3.0</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D7" t="n">
-        <v>50.0</v>
+        <v>1000.0</v>
       </c>
       <c r="E7" t="n">
-        <v>3400.0</v>
+        <v>2500.0</v>
       </c>
       <c r="F7" t="n">
         <v>4000.0</v>
       </c>
       <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" t="s">
         <v>31</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" ht="20.0" customHeight="true">
@@ -428,40 +463,43 @@
         <v>4.0</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D8" t="n">
-        <v>90.0</v>
+        <v>50.0</v>
       </c>
       <c r="E8" t="n">
-        <v>2000.0</v>
+        <v>3400.0</v>
       </c>
       <c r="F8" t="n">
-        <v>3500.0</v>
+        <v>4000.0</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I8" t="n">
-        <v>30.0</v>
+        <v>12.0</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M8" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" ht="20.0" customHeight="true">
@@ -469,40 +507,43 @@
         <v>5.0</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D9" t="n">
-        <v>120.0</v>
+        <v>90.0</v>
       </c>
       <c r="E9" t="n">
-        <v>2200.0</v>
+        <v>2000.0</v>
       </c>
       <c r="F9" t="n">
-        <v>3000.0</v>
+        <v>3500.0</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="I9" t="n">
-        <v>5.0</v>
+        <v>30.0</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M9" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="N9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" ht="20.0" customHeight="true">
@@ -510,40 +551,43 @@
         <v>6.0</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D10" t="n">
-        <v>90.0</v>
+        <v>120.0</v>
       </c>
       <c r="E10" t="n">
-        <v>1500.0</v>
+        <v>2200.0</v>
       </c>
       <c r="F10" t="n">
-        <v>2000.0</v>
+        <v>3000.0</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I10" t="n">
-        <v>16.0</v>
+        <v>5.0</v>
       </c>
       <c r="J10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="K10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="L10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="M10" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" ht="20.0" customHeight="true">
@@ -551,40 +595,43 @@
         <v>7.0</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D11" t="n">
-        <v>100.0</v>
+        <v>90.0</v>
       </c>
       <c r="E11" t="n">
-        <v>600.0</v>
+        <v>1500.0</v>
       </c>
       <c r="F11" t="n">
         <v>2000.0</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I11" t="n">
-        <v>5.0</v>
+        <v>16.0</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="L11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M11" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="N11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" ht="20.0" customHeight="true">
@@ -592,40 +639,43 @@
         <v>8.0</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D12" t="n">
-        <v>80.0</v>
+        <v>100.0</v>
       </c>
       <c r="E12" t="n">
-        <v>1000.0</v>
+        <v>600.0</v>
       </c>
       <c r="F12" t="n">
-        <v>1500.0</v>
+        <v>2000.0</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H12" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="I12" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="J12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M12" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="N12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" ht="20.0" customHeight="true">
@@ -633,40 +683,87 @@
         <v>9.0</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D13" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1500.0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" ht="20.0" customHeight="true">
+      <c r="A14" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="n">
         <v>70.0</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E14" t="n">
         <v>900.0</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F14" t="n">
         <v>1000.0</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" t="s">
         <v>31</v>
-      </c>
-      <c r="H13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" t="s">
-        <v>63</v>
-      </c>
-      <c r="M13" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sửa lại dữ liệu SPCT trong sql
</commit_message>
<xml_diff>
--- a/Dien_May_Do/src/com/dienmaydo/excel/SPCT.xlsx
+++ b/Dien_May_Do/src/com/dienmaydo/excel/SPCT.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
   <si>
     <t/>
   </si>
@@ -110,6 +110,9 @@
     <t>Đang kinh doanh</t>
   </si>
   <si>
+    <t>SPCT012</t>
+  </si>
+  <si>
     <t>SPCT02</t>
   </si>
   <si>
@@ -221,7 +224,28 @@
     <t>EWE451LB-DPX2</t>
   </si>
   <si>
+    <t>Cà rốt</t>
+  </si>
+  <si>
+    <t>11.0 - 33.0 - 22.0</t>
+  </si>
+  <si>
+    <t>Đá sức mạnh</t>
+  </si>
+  <si>
     <t>binhnonglanh.png</t>
+  </si>
+  <si>
+    <t>SPCT11</t>
+  </si>
+  <si>
+    <t>Inverter 11</t>
+  </si>
+  <si>
+    <t>SPCT13</t>
+  </si>
+  <si>
+    <t>Đá thời gian</t>
   </si>
 </sst>
 </file>
@@ -229,18 +253,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="16.0"/>
-      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -271,7 +290,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A3:N14"/>
+  <dimension ref="A3:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -422,34 +441,34 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D7" t="n">
-        <v>1000.0</v>
+        <v>32.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2500.0</v>
+        <v>141200.0</v>
       </c>
       <c r="F7" t="n">
-        <v>4000.0</v>
+        <v>54300.0</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I7" t="n">
-        <v>2.0</v>
+        <v>20.0</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="K7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="M7" t="s">
         <v>23</v>
@@ -463,43 +482,43 @@
         <v>4.0</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D8" t="n">
-        <v>50.0</v>
+        <v>1000.0</v>
       </c>
       <c r="E8" t="n">
-        <v>3400.0</v>
+        <v>2500.0</v>
       </c>
       <c r="F8" t="n">
         <v>4000.0</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I8" t="n">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M8" t="s">
         <v>23</v>
       </c>
       <c r="N8" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" ht="20.0" customHeight="true">
@@ -507,37 +526,37 @@
         <v>5.0</v>
       </c>
       <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3400.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" t="s">
         <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" t="n">
-        <v>90.0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2000.0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3500.0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" t="s">
-        <v>48</v>
       </c>
       <c r="M9" t="s">
         <v>23</v>
@@ -551,37 +570,37 @@
         <v>6.0</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D10" t="n">
-        <v>120.0</v>
+        <v>90.0</v>
       </c>
       <c r="E10" t="n">
-        <v>2200.0</v>
+        <v>2000.0</v>
       </c>
       <c r="F10" t="n">
-        <v>3000.0</v>
+        <v>3500.0</v>
       </c>
       <c r="G10" t="s">
         <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="I10" t="n">
-        <v>5.0</v>
+        <v>30.0</v>
       </c>
       <c r="J10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="M10" t="s">
         <v>23</v>
@@ -595,43 +614,43 @@
         <v>7.0</v>
       </c>
       <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2200.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3000.0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" t="n">
-        <v>90.0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1500.0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2000.0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11" t="s">
-        <v>57</v>
-      </c>
-      <c r="L11" t="s">
-        <v>58</v>
-      </c>
       <c r="M11" t="s">
         <v>23</v>
       </c>
       <c r="N11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" ht="20.0" customHeight="true">
@@ -639,37 +658,37 @@
         <v>8.0</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D12" t="n">
-        <v>100.0</v>
+        <v>90.0</v>
       </c>
       <c r="E12" t="n">
-        <v>600.0</v>
+        <v>1500.0</v>
       </c>
       <c r="F12" t="n">
         <v>2000.0</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I12" t="n">
-        <v>5.0</v>
+        <v>16.0</v>
       </c>
       <c r="J12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K12" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="L12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M12" t="s">
         <v>23</v>
@@ -683,37 +702,37 @@
         <v>9.0</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D13" t="n">
-        <v>80.0</v>
+        <v>100.0</v>
       </c>
       <c r="E13" t="n">
-        <v>1000.0</v>
+        <v>600.0</v>
       </c>
       <c r="F13" t="n">
-        <v>1500.0</v>
+        <v>2000.0</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="I13" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K13" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="L13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M13" t="s">
         <v>23</v>
@@ -727,42 +746,174 @@
         <v>10.0</v>
       </c>
       <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1500.0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" t="s">
         <v>67</v>
       </c>
-      <c r="C14" t="s">
+      <c r="M14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" ht="20.0" customHeight="true">
+      <c r="A15" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B15" t="s">
         <v>68</v>
       </c>
-      <c r="D14" t="n">
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="n">
         <v>70.0</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E15" t="n">
         <v>900.0</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F15" t="n">
         <v>1000.0</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>27</v>
       </c>
-      <c r="H14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" t="n">
+      <c r="H15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" t="n">
         <v>20.0</v>
       </c>
-      <c r="J14" t="s">
-        <v>29</v>
-      </c>
-      <c r="K14" t="s">
-        <v>47</v>
-      </c>
-      <c r="L14" t="s">
-        <v>69</v>
-      </c>
-      <c r="M14" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="J15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" t="s">
+        <v>72</v>
+      </c>
+      <c r="L15" t="s">
+        <v>73</v>
+      </c>
+      <c r="M15" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" ht="20.0" customHeight="true">
+      <c r="A16" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1100.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>31100.0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" t="s">
+        <v>72</v>
+      </c>
+      <c r="L16" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" ht="20.0" customHeight="true">
+      <c r="A17" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2500.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" t="s">
+        <v>77</v>
+      </c>
+      <c r="L17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update lại đường dẫn xuất file excel/SPCT.xlsx
</commit_message>
<xml_diff>
--- a/Dien_May_Do/src/com/dienmaydo/excel/SPCT.xlsx
+++ b/Dien_May_Do/src/com/dienmaydo/excel/SPCT.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="75">
   <si>
     <t/>
   </si>
@@ -62,147 +62,159 @@
     <t>Trạng thái</t>
   </si>
   <si>
+    <t>BnCN01</t>
+  </si>
+  <si>
+    <t>Bình nóng BB</t>
+  </si>
+  <si>
+    <t>Không phổ biến</t>
+  </si>
+  <si>
+    <t>Đỏ</t>
+  </si>
+  <si>
+    <t>82.0 - 20.5 - 48.2</t>
+  </si>
+  <si>
+    <t>Kính cường lực</t>
+  </si>
+  <si>
+    <t>132803876_405165884152273_5076209746959171268_n.jpg</t>
+  </si>
+  <si>
+    <t>Bình nóng CC</t>
+  </si>
+  <si>
+    <t>Đang kinh doanh</t>
+  </si>
+  <si>
+    <t>BnlT01</t>
+  </si>
+  <si>
+    <t>Bình nóng lạnh Test</t>
+  </si>
+  <si>
+    <t>Phổ biến</t>
+  </si>
+  <si>
+    <t>Trắng đen</t>
+  </si>
+  <si>
+    <t>77.0 - 77.0 - 77.0</t>
+  </si>
+  <si>
+    <t>Thép không gỉ, Kim loại phủ sơn tĩnh điện</t>
+  </si>
+  <si>
+    <t>hiennv.png</t>
+  </si>
+  <si>
+    <t>Bình nóng lạnh Test Bình nóng lạnh Test</t>
+  </si>
+  <si>
     <t>SPCT01</t>
   </si>
   <si>
     <t>AH-X9XEW</t>
   </si>
   <si>
-    <t>Không phổ biến</t>
-  </si>
-  <si>
     <t>Trắng</t>
   </si>
   <si>
     <t>74.0 - 25.5 - 48.2</t>
   </si>
   <si>
-    <t>Thép không gỉ, Kim loại phủ sơn tĩnh điện</t>
-  </si>
-  <si>
     <t>maylanh.png</t>
   </si>
   <si>
     <t>No Mô Tả</t>
   </si>
   <si>
-    <t>Ngừng kinh doanh</t>
-  </si>
-  <si>
-    <t>SPCT011</t>
-  </si>
-  <si>
-    <t>AH-X9XEW1</t>
-  </si>
-  <si>
-    <t>Phổ biến</t>
-  </si>
-  <si>
-    <t>Nâu</t>
-  </si>
-  <si>
-    <t>82.0 - 20.5 - 48.2</t>
+    <t>SPCT02</t>
+  </si>
+  <si>
+    <t>BM01</t>
+  </si>
+  <si>
+    <t>Đen</t>
+  </si>
+  <si>
+    <t>30.0 - 15.5 - 14.0</t>
+  </si>
+  <si>
+    <t>Thép không gỉ</t>
+  </si>
+  <si>
+    <t>loa.png</t>
+  </si>
+  <si>
+    <t>SPCT03</t>
+  </si>
+  <si>
+    <t>KG50F62</t>
+  </si>
+  <si>
+    <t>70.0 - 30.0 - 25.5</t>
+  </si>
+  <si>
+    <t>Kính nhựa</t>
+  </si>
+  <si>
+    <t>dieuhoa.png</t>
+  </si>
+  <si>
+    <t>SPCT04</t>
+  </si>
+  <si>
+    <t>FV1409S4W</t>
+  </si>
+  <si>
+    <t>80.0 - 70.5 - 104.7</t>
+  </si>
+  <si>
+    <t>Nhựa dẻo</t>
+  </si>
+  <si>
+    <t>maygiat.png</t>
+  </si>
+  <si>
+    <t>SPCT05</t>
+  </si>
+  <si>
+    <t>KD-43X75</t>
+  </si>
+  <si>
+    <t>90.0 - 5.0 - 70.0</t>
+  </si>
+  <si>
+    <t>Kim loại phủ sơn tĩnh điện</t>
+  </si>
+  <si>
+    <t>SPCT06</t>
+  </si>
+  <si>
+    <t>Inverter NR-BC360QKVN</t>
+  </si>
+  <si>
+    <t>70.0 - 65.0 - 150.0</t>
+  </si>
+  <si>
+    <t>tulanh.png</t>
+  </si>
+  <si>
+    <t>SPCT07</t>
+  </si>
+  <si>
+    <t>MC-CL575KN49 2000W</t>
+  </si>
+  <si>
+    <t>40.0 - 20.0 - 70.0</t>
   </si>
   <si>
     <t>Sắt không gỉ</t>
   </si>
   <si>
-    <t>Đang kinh doanh</t>
-  </si>
-  <si>
-    <t>SPCT012</t>
-  </si>
-  <si>
-    <t>SPCT02</t>
-  </si>
-  <si>
-    <t>BM01</t>
-  </si>
-  <si>
-    <t>Đen</t>
-  </si>
-  <si>
-    <t>30.0 - 15.5 - 14.0</t>
-  </si>
-  <si>
-    <t>Thép không gỉ</t>
-  </si>
-  <si>
-    <t>loa.png</t>
-  </si>
-  <si>
-    <t>SPCT03</t>
-  </si>
-  <si>
-    <t>KG50F62</t>
-  </si>
-  <si>
-    <t>70.0 - 30.0 - 25.5</t>
-  </si>
-  <si>
-    <t>Kính nhựa</t>
-  </si>
-  <si>
-    <t>dieuhoa.png</t>
-  </si>
-  <si>
-    <t>SPCT04</t>
-  </si>
-  <si>
-    <t>FV1409S4W</t>
-  </si>
-  <si>
-    <t>Trắng đen</t>
-  </si>
-  <si>
-    <t>80.0 - 70.5 - 104.7</t>
-  </si>
-  <si>
-    <t>Nhựa dẻo</t>
-  </si>
-  <si>
-    <t>maygiat.png</t>
-  </si>
-  <si>
-    <t>SPCT05</t>
-  </si>
-  <si>
-    <t>KD-43X75</t>
-  </si>
-  <si>
-    <t>90.0 - 5.0 - 70.0</t>
-  </si>
-  <si>
-    <t>Kim loại phủ sơn tĩnh điện</t>
-  </si>
-  <si>
-    <t>tivi.png</t>
-  </si>
-  <si>
-    <t>SPCT06</t>
-  </si>
-  <si>
-    <t>Inverter NR-BC360QKVN</t>
-  </si>
-  <si>
-    <t>70.0 - 65.0 - 150.0</t>
-  </si>
-  <si>
-    <t>Kính cường lực</t>
-  </si>
-  <si>
-    <t>tulanh.png</t>
-  </si>
-  <si>
-    <t>SPCT07</t>
-  </si>
-  <si>
-    <t>MC-CL575KN49 2000W</t>
-  </si>
-  <si>
-    <t>40.0 - 20.0 - 70.0</t>
-  </si>
-  <si>
     <t>mayhutbui.png</t>
   </si>
   <si>
@@ -224,28 +236,7 @@
     <t>EWE451LB-DPX2</t>
   </si>
   <si>
-    <t>Cà rốt</t>
-  </si>
-  <si>
-    <t>11.0 - 33.0 - 22.0</t>
-  </si>
-  <si>
-    <t>Đá sức mạnh</t>
-  </si>
-  <si>
     <t>binhnonglanh.png</t>
-  </si>
-  <si>
-    <t>SPCT11</t>
-  </si>
-  <si>
-    <t>Inverter 11</t>
-  </si>
-  <si>
-    <t>SPCT13</t>
-  </si>
-  <si>
-    <t>Đá thời gian</t>
   </si>
 </sst>
 </file>
@@ -290,7 +281,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A3:N17"/>
+  <dimension ref="A3:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -356,13 +347,13 @@
         <v>17</v>
       </c>
       <c r="D5" t="n">
-        <v>100.0</v>
+        <v>22.0</v>
       </c>
       <c r="E5" t="n">
-        <v>2000.0</v>
+        <v>33.0</v>
       </c>
       <c r="F5" t="n">
-        <v>3000.0</v>
+        <v>44.0</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -371,7 +362,7 @@
         <v>19</v>
       </c>
       <c r="I5" t="n">
-        <v>20.0</v>
+        <v>7.0</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
@@ -400,13 +391,13 @@
         <v>26</v>
       </c>
       <c r="D6" t="n">
-        <v>32.0</v>
+        <v>11.0</v>
       </c>
       <c r="E6" t="n">
-        <v>141200.0</v>
+        <v>22.0</v>
       </c>
       <c r="F6" t="n">
-        <v>54300.0</v>
+        <v>33.0</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -424,13 +415,13 @@
         <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="N6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" ht="20.0" customHeight="true">
@@ -438,43 +429,43 @@
         <v>3.0</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D7" t="n">
-        <v>32.0</v>
+        <v>10.0</v>
       </c>
       <c r="E7" t="n">
-        <v>141200.0</v>
+        <v>900000.0</v>
       </c>
       <c r="F7" t="n">
-        <v>54300.0</v>
+        <v>1200000.0</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I7" t="n">
         <v>20.0</v>
       </c>
       <c r="J7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="K7" t="s">
         <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="M7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" ht="20.0" customHeight="true">
@@ -482,43 +473,43 @@
         <v>4.0</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D8" t="n">
-        <v>1000.0</v>
+        <v>10.0</v>
       </c>
       <c r="E8" t="n">
-        <v>2500.0</v>
+        <v>100000.0</v>
       </c>
       <c r="F8" t="n">
-        <v>4000.0</v>
+        <v>200000.0</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I8" t="n">
         <v>2.0</v>
       </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="K8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" t="s">
         <v>38</v>
       </c>
-      <c r="M8" t="s">
-        <v>23</v>
-      </c>
       <c r="N8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" ht="20.0" customHeight="true">
@@ -526,40 +517,40 @@
         <v>5.0</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D9" t="n">
-        <v>50.0</v>
+        <v>10.0</v>
       </c>
       <c r="E9" t="n">
-        <v>3400.0</v>
+        <v>950000.0</v>
       </c>
       <c r="F9" t="n">
-        <v>4000.0</v>
+        <v>1500000.0</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I9" t="n">
         <v>12.0</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="M9" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N9" t="s">
         <v>24</v>
@@ -570,40 +561,40 @@
         <v>6.0</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D10" t="n">
-        <v>90.0</v>
+        <v>10.0</v>
       </c>
       <c r="E10" t="n">
-        <v>2000.0</v>
+        <v>800000.0</v>
       </c>
       <c r="F10" t="n">
-        <v>3500.0</v>
+        <v>950000.0</v>
       </c>
       <c r="G10" t="s">
         <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="I10" t="n">
         <v>30.0</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L10" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="M10" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N10" t="s">
         <v>24</v>
@@ -614,40 +605,40 @@
         <v>7.0</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D11" t="n">
-        <v>120.0</v>
+        <v>10.0</v>
       </c>
       <c r="E11" t="n">
-        <v>2200.0</v>
+        <v>1700000.0</v>
       </c>
       <c r="F11" t="n">
-        <v>3000.0</v>
+        <v>2100000.0</v>
       </c>
       <c r="G11" t="s">
         <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I11" t="n">
         <v>5.0</v>
       </c>
       <c r="J11" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="K11" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="L11" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="M11" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N11" t="s">
         <v>24</v>
@@ -658,43 +649,43 @@
         <v>8.0</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D12" t="n">
-        <v>90.0</v>
+        <v>10.0</v>
       </c>
       <c r="E12" t="n">
-        <v>1500.0</v>
+        <v>400000.0</v>
       </c>
       <c r="F12" t="n">
-        <v>2000.0</v>
+        <v>650000.0</v>
       </c>
       <c r="G12" t="s">
         <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="I12" t="n">
         <v>16.0</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="K12" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M12" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" ht="20.0" customHeight="true">
@@ -702,43 +693,43 @@
         <v>9.0</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D13" t="n">
-        <v>100.0</v>
+        <v>10.0</v>
       </c>
       <c r="E13" t="n">
-        <v>600.0</v>
+        <v>100000.0</v>
       </c>
       <c r="F13" t="n">
-        <v>2000.0</v>
+        <v>280000.0</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="I13" t="n">
         <v>5.0</v>
       </c>
       <c r="J13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K13" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="L13" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="M13" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" ht="20.0" customHeight="true">
@@ -746,43 +737,43 @@
         <v>10.0</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D14" t="n">
-        <v>80.0</v>
+        <v>10.0</v>
       </c>
       <c r="E14" t="n">
-        <v>1000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="F14" t="n">
-        <v>1500.0</v>
+        <v>250000.0</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I14" t="n">
         <v>7.0</v>
       </c>
       <c r="J14" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K14" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="L14" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="M14" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N14" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" ht="20.0" customHeight="true">
@@ -790,131 +781,43 @@
         <v>11.0</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D15" t="n">
-        <v>70.0</v>
+        <v>10.0</v>
       </c>
       <c r="E15" t="n">
-        <v>900.0</v>
+        <v>90000.0</v>
       </c>
       <c r="F15" t="n">
-        <v>1000.0</v>
+        <v>150000.0</v>
       </c>
       <c r="G15" t="s">
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="I15" t="n">
         <v>20.0</v>
       </c>
       <c r="J15" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="K15" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="L15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M15" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" ht="20.0" customHeight="true">
-      <c r="A16" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1100.0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>31100.0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>71</v>
-      </c>
-      <c r="K16" t="s">
-        <v>72</v>
-      </c>
-      <c r="L16" t="s">
-        <v>38</v>
-      </c>
-      <c r="M16" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" ht="20.0" customHeight="true">
-      <c r="A17" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>2500.0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>4000.0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" t="s">
-        <v>77</v>
-      </c>
-      <c r="L17" t="s">
-        <v>38</v>
-      </c>
-      <c r="M17" t="s">
-        <v>23</v>
-      </c>
-      <c r="N17" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>